<commit_message>
(just some stuff I forgot to commit oop)
</commit_message>
<xml_diff>
--- a/VaultViewer/VaultViewer/DataAccessLayer/Data/AdminData.xlsx
+++ b/VaultViewer/VaultViewer/DataAccessLayer/Data/AdminData.xlsx
@@ -25,6 +25,15 @@
     <x:t>EmployeeID</x:t>
   </x:si>
   <x:si>
+    <x:t>Artyom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2a$11$fethBIsQ2NFmRQHECCLp8u48zXU973BxPYeRLklkHt.1GyYJ4I1Yq</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
     <x:t>Admin</x:t>
   </x:si>
   <x:si>
@@ -32,51 +41,6 @@
   </x:si>
   <x:si>
     <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Artyom</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2a$11$fethBIsQ2NFmRQHECCLp8u48zXU973BxPYeRLklkHt.1GyYJ4I1Yq</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Elliot</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2a$11$.QeINrO0EsiV5n5cXZ.ql.TrEmXmpk2szYo/EpVFi7MmoAEXvRPEK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2a$11$BAdFSraqs/4z6yaNcftwo.ciYMFjaGavyjnQnX7dwjyAk/7ot3fBe</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HumanResources</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2a$11$2n3zO5EkQPXxk1sPubn07.UBolyLpLFmodH7RY02VvCh/CDoKunbW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2a$11$lcxaghH.VJGXjgjTFWQt3ON31xQdnJydtLd2be9qdHMZzjrj6WBuO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -427,7 +391,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C7"/>
+  <x:dimension ref="A1:C3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -464,50 +428,6 @@
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3">
-      <x:c r="A7" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>